<commit_message>
one step closer to end
</commit_message>
<xml_diff>
--- a/UDP_navrh_hlavicky.xlsx
+++ b/UDP_navrh_hlavicky.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb762f2072cc6c8f/Počítač/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb762f2072cc6c8f/Počítač/testfolder/PKS_UDP_kom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76BB44A2-FBBB-42A0-8756-688615391B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{76BB44A2-FBBB-42A0-8756-688615391B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CBE6579-FDCD-46DE-8465-EB426A88DC8E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{B9CB759D-126A-43C7-97B1-F08CC51E13FB}"/>
   </bookViews>
@@ -36,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Message Type</t>
-  </si>
-  <si>
-    <t>Flags</t>
-  </si>
-  <si>
-    <t>32b</t>
-  </si>
-  <si>
-    <t>1B</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Checksum</t>
   </si>
@@ -66,6 +54,9 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Message Type + Flags</t>
   </si>
 </sst>
 </file>
@@ -104,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -179,11 +170,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,9 +205,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -206,10 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -221,7 +226,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -239,6 +247,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -558,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5DEBC1-C962-4CB6-9A68-4BAFFA5F1EC2}">
-  <dimension ref="C2:AK7"/>
+  <dimension ref="C2:AH7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ7" sqref="AJ7"/>
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.54296875" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -569,77 +581,85 @@
     <col min="1" max="16384" width="4.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:37" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="M2" s="5">
-        <v>1</v>
-      </c>
-      <c r="N2" s="5">
-        <v>1</v>
-      </c>
-      <c r="O2" s="5">
-        <v>1</v>
-      </c>
-      <c r="P2" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>1</v>
-      </c>
-      <c r="R2" s="5">
-        <v>1</v>
-      </c>
-      <c r="S2" s="5">
-        <v>1</v>
-      </c>
-      <c r="T2" s="5">
-        <v>1</v>
-      </c>
-      <c r="U2" s="5">
-        <v>1</v>
-      </c>
-      <c r="V2" s="5">
-        <v>1</v>
-      </c>
-      <c r="W2" s="5">
-        <v>2</v>
-      </c>
-      <c r="X2" s="5">
-        <v>2</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="5">
-        <v>2</v>
-      </c>
-      <c r="AC2" s="5">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="5">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="5">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="5">
-        <v>2</v>
-      </c>
-      <c r="AG2" s="5">
+    <row r="2" spans="3:34" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>1</v>
+      </c>
+      <c r="R2" s="4">
+        <v>1</v>
+      </c>
+      <c r="S2" s="4">
+        <v>1</v>
+      </c>
+      <c r="T2" s="4">
+        <v>1</v>
+      </c>
+      <c r="U2" s="4">
+        <v>1</v>
+      </c>
+      <c r="V2" s="4">
+        <v>1</v>
+      </c>
+      <c r="W2" s="4">
+        <v>2</v>
+      </c>
+      <c r="X2" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="4">
         <v>3</v>
       </c>
-      <c r="AH2" s="5">
+      <c r="AH2" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:37" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:34" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="2">
         <v>0</v>
       </c>
@@ -661,13 +681,13 @@
       <c r="I3" s="1">
         <v>6</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>7</v>
       </c>
       <c r="K3" s="1">
         <v>8</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="1">
         <v>9</v>
       </c>
       <c r="M3" s="1">
@@ -685,7 +705,7 @@
       <c r="Q3" s="1">
         <v>4</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="5">
         <v>5</v>
       </c>
       <c r="S3" s="1">
@@ -697,7 +717,7 @@
       <c r="U3" s="1">
         <v>8</v>
       </c>
-      <c r="V3" s="8">
+      <c r="V3" s="1">
         <v>9</v>
       </c>
       <c r="W3" s="1">
@@ -709,7 +729,7 @@
       <c r="Y3" s="1">
         <v>2</v>
       </c>
-      <c r="Z3" s="6">
+      <c r="Z3" s="5">
         <v>3</v>
       </c>
       <c r="AA3" s="1">
@@ -727,151 +747,143 @@
       <c r="AE3" s="1">
         <v>8</v>
       </c>
-      <c r="AF3" s="8">
+      <c r="AF3" s="1">
         <v>9</v>
       </c>
       <c r="AG3" s="1">
         <v>0</v>
       </c>
-      <c r="AH3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK3" s="9" t="s">
+      <c r="AH3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:34" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="10"/>
+    </row>
+    <row r="5" spans="3:34" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
     </row>
-    <row r="4" spans="3:37" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="10" t="s">
+    <row r="6" spans="3:34" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="12"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="10"/>
     </row>
-    <row r="5" spans="3:37" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-    </row>
-    <row r="6" spans="3:37" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="13"/>
-    </row>
-    <row r="7" spans="3:37" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="3:34" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C2:L2"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="K5:R5"/>
     <mergeCell ref="S5:AH5"/>
     <mergeCell ref="C6:AH6"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
     <mergeCell ref="K4:Z4"/>
     <mergeCell ref="AA4:AH4"/>
+    <mergeCell ref="C4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>